<commit_message>
creating small blending problem. Fixing some constraints, adding excel report
</commit_message>
<xml_diff>
--- a/pareto/case_studies/blending_problem.xlsx
+++ b/pareto/case_studies/blending_problem.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54325818ffabb65a/Documents/KeyLogic/PARETO/project-pareto/pareto/case_studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="400" documentId="13_ncr:1_{2082DF02-1D44-481C-BCA6-29895472D724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F97C2BC8-E87C-4CD0-B6D6-028E3929E59D}"/>
+  <xr:revisionPtr revIDLastSave="487" documentId="13_ncr:1_{2082DF02-1D44-481C-BCA6-29895472D724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDB800A2-FF39-446E-AEBC-5E7E5B79EDFB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="892" firstSheet="15" activeTab="23" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="892" firstSheet="12" activeTab="17" xr2:uid="{FB8C51AB-905F-4544-9E4B-1F4384FA855C}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="33" r:id="rId1"/>
@@ -26,17 +26,16 @@
     <sheet name="TransportMode" sheetId="101" r:id="rId11"/>
     <sheet name="TimePeriods" sheetId="102" r:id="rId12"/>
     <sheet name="Topology" sheetId="100" r:id="rId13"/>
-    <sheet name="CompletionsDemand" sheetId="8" r:id="rId14"/>
-    <sheet name="CustomersDemand" sheetId="103" r:id="rId15"/>
-    <sheet name="DisposalCost" sheetId="111" r:id="rId16"/>
-    <sheet name="FreshWaterAvailability" sheetId="104" r:id="rId17"/>
-    <sheet name="FreshWaterCost" sheetId="110" r:id="rId18"/>
-    <sheet name="StorageCapacity" sheetId="105" r:id="rId19"/>
-    <sheet name="StorageInit" sheetId="109" r:id="rId20"/>
-    <sheet name="TransportCapacity" sheetId="106" r:id="rId21"/>
-    <sheet name="TransportCost" sheetId="108" r:id="rId22"/>
-    <sheet name="TransportDistances" sheetId="107" r:id="rId23"/>
-    <sheet name="WaterProfiles" sheetId="65" r:id="rId24"/>
+    <sheet name="Demand" sheetId="8" r:id="rId14"/>
+    <sheet name="DisposalCost" sheetId="111" r:id="rId15"/>
+    <sheet name="FreshWaterAvailability" sheetId="104" r:id="rId16"/>
+    <sheet name="FreshWaterCost" sheetId="110" r:id="rId17"/>
+    <sheet name="StorageCapacity" sheetId="105" r:id="rId18"/>
+    <sheet name="StorageInit" sheetId="109" r:id="rId19"/>
+    <sheet name="TransportCapacity" sheetId="106" r:id="rId20"/>
+    <sheet name="TransportCost" sheetId="108" r:id="rId21"/>
+    <sheet name="TransportDistances" sheetId="107" r:id="rId22"/>
+    <sheet name="WaterProfiles" sheetId="65" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="116">
   <si>
     <t>List of all Production Pad Identifiers [-]</t>
   </si>
@@ -365,9 +364,6 @@
     <t>TransportMode</t>
   </si>
   <si>
-    <t>Customers</t>
-  </si>
-  <si>
     <t>Table of Fresh Water availability [bbl/week]</t>
   </si>
   <si>
@@ -378,9 +374,6 @@
   </si>
   <si>
     <t>Table of Disposal Operational Cost  [$/bbl]</t>
-  </si>
-  <si>
-    <t>Table of Customers Water Demand for Completions Sites over Weeks [bbl/day]</t>
   </si>
   <si>
     <t>List of all Customers Identifiers [-]</t>
@@ -890,10 +883,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1855,7 +1844,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -1915,7 +1904,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
@@ -1986,7 +1975,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1997,7 +1986,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -2082,9 +2071,15 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="G3" s="7">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7">
+        <v>1</v>
+      </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
@@ -2111,15 +2106,17 @@
       <c r="B4" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="7">
-        <v>1</v>
-      </c>
+      <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
       <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="I4" s="7">
+        <v>1</v>
+      </c>
       <c r="J4" s="7"/>
       <c r="K4" s="7">
         <v>1</v>
@@ -2146,14 +2143,14 @@
       <c r="B5" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="7">
-        <v>1</v>
-      </c>
+      <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="H5" s="7">
+        <v>1</v>
+      </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -2179,16 +2176,16 @@
       <c r="B6" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="7">
-        <v>1</v>
-      </c>
+      <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="J6" s="7">
+        <v>1</v>
+      </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
@@ -2220,13 +2217,19 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+      <c r="K7" s="7">
+        <v>1</v>
+      </c>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
+      <c r="O7" s="7">
+        <v>1</v>
+      </c>
       <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
+      <c r="Q7" s="7">
+        <v>1</v>
+      </c>
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
@@ -2283,7 +2286,9 @@
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
+      <c r="N9" s="7">
+        <v>1</v>
+      </c>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
@@ -2310,14 +2315,18 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
+      <c r="L10" s="7">
+        <v>1</v>
+      </c>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
+      <c r="S10" s="7">
+        <v>1</v>
+      </c>
       <c r="T10" s="7"/>
       <c r="U10" s="7"/>
       <c r="V10" s="7"/>
@@ -2334,18 +2343,24 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="G11" s="7">
+        <v>1</v>
+      </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
+      <c r="N11" s="7">
+        <v>1</v>
+      </c>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
+      <c r="R11" s="7">
+        <v>1</v>
+      </c>
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
       <c r="U11" s="7"/>
@@ -2366,15 +2381,21 @@
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
+      <c r="J12" s="7">
+        <v>1</v>
+      </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
+      <c r="P12" s="7">
+        <v>1</v>
+      </c>
       <c r="Q12" s="7"/>
-      <c r="R12" s="7"/>
+      <c r="R12" s="7">
+        <v>1</v>
+      </c>
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
       <c r="U12" s="7"/>
@@ -2388,10 +2409,18 @@
       <c r="B13" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
+      <c r="C13" s="7">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7">
+        <v>1</v>
+      </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
@@ -2423,9 +2452,13 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="I14" s="7">
+        <v>1</v>
+      </c>
       <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
+      <c r="K14" s="7">
+        <v>1</v>
+      </c>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
@@ -2450,8 +2483,12 @@
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="G15" s="7">
+        <v>1</v>
+      </c>
+      <c r="H15" s="7">
+        <v>1</v>
+      </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
@@ -2459,7 +2496,9 @@
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
+      <c r="P15" s="7">
+        <v>1</v>
+      </c>
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
       <c r="S15" s="7"/>
@@ -2484,12 +2523,18 @@
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
+      <c r="L16" s="7">
+        <v>1</v>
+      </c>
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
+      <c r="O16" s="7">
+        <v>1</v>
+      </c>
       <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
+      <c r="Q16" s="7">
+        <v>1</v>
+      </c>
       <c r="R16" s="7"/>
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
@@ -2508,7 +2553,9 @@
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+      <c r="G17" s="7">
+        <v>1</v>
+      </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -2517,9 +2564,13 @@
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
+      <c r="P17" s="7">
+        <v>1</v>
+      </c>
       <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
+      <c r="R17" s="7">
+        <v>1</v>
+      </c>
       <c r="S17" s="7"/>
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
@@ -2541,16 +2592,24 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
+      <c r="K18" s="7">
+        <v>1</v>
+      </c>
+      <c r="L18" s="7">
+        <v>1</v>
+      </c>
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
+      <c r="Q18" s="7">
+        <v>1</v>
+      </c>
       <c r="R18" s="7"/>
       <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
+      <c r="T18" s="7">
+        <v>1</v>
+      </c>
       <c r="U18" s="7"/>
       <c r="V18" s="7"/>
       <c r="W18" s="29"/>
@@ -2569,9 +2628,13 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
+      <c r="J19" s="7">
+        <v>1</v>
+      </c>
       <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
+      <c r="L19" s="7">
+        <v>1</v>
+      </c>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
@@ -2633,9 +2696,7 @@
       <c r="I21" s="7">
         <v>1</v>
       </c>
-      <c r="J21" s="7">
-        <v>1</v>
-      </c>
+      <c r="J21" s="7"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
@@ -2661,18 +2722,12 @@
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
-      <c r="G22" s="7">
-        <v>1</v>
-      </c>
+      <c r="G22" s="7"/>
       <c r="H22" s="7">
         <v>1</v>
       </c>
-      <c r="I22" s="7">
-        <v>1</v>
-      </c>
-      <c r="J22" s="7">
-        <v>1</v>
-      </c>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
       <c r="K22" s="7"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
@@ -2698,15 +2753,9 @@
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
-      <c r="G23" s="8">
-        <v>1</v>
-      </c>
-      <c r="H23" s="8">
-        <v>1</v>
-      </c>
-      <c r="I23" s="8">
-        <v>1</v>
-      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
       <c r="J23" s="8">
         <v>1</v>
       </c>
@@ -2855,9 +2904,7 @@
       <c r="B28" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="7">
-        <v>1</v>
-      </c>
+      <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -2888,9 +2935,7 @@
       <c r="B29" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="7">
-        <v>1</v>
-      </c>
+      <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -2921,9 +2966,7 @@
       <c r="B30" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="7">
-        <v>1</v>
-      </c>
+      <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -2954,9 +2997,7 @@
       <c r="B31" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="7">
-        <v>1</v>
-      </c>
+      <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -3107,18 +3148,10 @@
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
-      <c r="G36" s="7">
-        <v>1</v>
-      </c>
-      <c r="H36" s="7">
-        <v>1</v>
-      </c>
-      <c r="I36" s="7">
-        <v>1</v>
-      </c>
-      <c r="J36" s="7">
-        <v>1</v>
-      </c>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
@@ -3144,18 +3177,10 @@
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
-      <c r="G37" s="7">
-        <v>1</v>
-      </c>
-      <c r="H37" s="7">
-        <v>1</v>
-      </c>
-      <c r="I37" s="7">
-        <v>1</v>
-      </c>
-      <c r="J37" s="7">
-        <v>1</v>
-      </c>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
       <c r="K37" s="7"/>
       <c r="L37" s="7"/>
       <c r="M37" s="7"/>
@@ -3181,18 +3206,10 @@
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
-      <c r="G38" s="8">
-        <v>1</v>
-      </c>
-      <c r="H38" s="8">
-        <v>1</v>
-      </c>
-      <c r="I38" s="8">
-        <v>1</v>
-      </c>
-      <c r="J38" s="8">
-        <v>1</v>
-      </c>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
@@ -3218,7 +3235,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" activeCellId="1" sqref="B3 B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3264,7 +3281,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="36">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="C3" s="36"/>
       <c r="D3" s="36"/>
@@ -3278,7 +3295,7 @@
         <v>80</v>
       </c>
       <c r="B4" s="36">
-        <v>400000</v>
+        <v>500000</v>
       </c>
       <c r="C4" s="36">
         <v>450000</v>
@@ -3294,10 +3311,10 @@
         <v>81</v>
       </c>
       <c r="B5" s="36">
-        <v>600000</v>
+        <v>300000</v>
       </c>
       <c r="C5" s="36">
-        <v>650000</v>
+        <v>300000</v>
       </c>
       <c r="D5" s="36">
         <v>300000</v>
@@ -3312,16 +3329,40 @@
         <v>82</v>
       </c>
       <c r="B6" s="31">
-        <v>500000</v>
+        <v>400000</v>
       </c>
       <c r="C6" s="31">
-        <v>500000</v>
+        <v>400000</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="31"/>
       <c r="F6" s="31"/>
       <c r="G6" s="31"/>
       <c r="H6" s="32"/>
+    </row>
+    <row r="7" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31">
+        <v>10000</v>
+      </c>
+      <c r="D7" s="31">
+        <v>10000</v>
+      </c>
+      <c r="E7" s="31">
+        <v>10000</v>
+      </c>
+      <c r="F7" s="31">
+        <v>10000</v>
+      </c>
+      <c r="G7" s="31">
+        <v>10000</v>
+      </c>
+      <c r="H7" s="32">
+        <v>10000</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D9" s="2"/>
@@ -3376,125 +3417,6 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE232A6-095C-4682-9EB4-225655171DE4}">
-  <dimension ref="A1:H14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="6" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31">
-        <v>10000</v>
-      </c>
-      <c r="D3" s="31">
-        <v>10000</v>
-      </c>
-      <c r="E3" s="31">
-        <v>10000</v>
-      </c>
-      <c r="F3" s="31">
-        <v>10000</v>
-      </c>
-      <c r="G3" s="31">
-        <v>10000</v>
-      </c>
-      <c r="H3" s="32">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C103B193-705C-4271-A3F0-6E7CCF41829E}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3510,7 +3432,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3535,12 +3457,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E306EF86-D95D-4D95-A346-E512C46BF2E3}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3554,7 +3476,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3588,25 +3510,25 @@
         <v>65</v>
       </c>
       <c r="B3" s="36">
-        <v>350000</v>
+        <v>900000</v>
       </c>
       <c r="C3" s="36">
-        <v>350000</v>
+        <v>900000</v>
       </c>
       <c r="D3" s="36">
-        <v>350000</v>
+        <v>900000</v>
       </c>
       <c r="E3" s="36">
-        <v>350000</v>
+        <v>900000</v>
       </c>
       <c r="F3" s="36">
-        <v>350000</v>
+        <v>900000</v>
       </c>
       <c r="G3" s="36">
-        <v>350000</v>
+        <v>900000</v>
       </c>
       <c r="H3" s="30">
-        <v>350000</v>
+        <v>900000</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3640,25 +3562,25 @@
         <v>84</v>
       </c>
       <c r="B5" s="31">
-        <v>560000</v>
+        <v>800000</v>
       </c>
       <c r="C5" s="31">
-        <v>560000</v>
+        <v>800000</v>
       </c>
       <c r="D5" s="31">
-        <v>560000</v>
+        <v>800000</v>
       </c>
       <c r="E5" s="31">
-        <v>560000</v>
+        <v>800000</v>
       </c>
       <c r="F5" s="31">
-        <v>560000</v>
+        <v>800000</v>
       </c>
       <c r="G5" s="31">
-        <v>560000</v>
+        <v>800000</v>
       </c>
       <c r="H5" s="32">
-        <v>560000</v>
+        <v>800000</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -3677,7 +3599,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F577E3C0-784C-4861-A323-2A87B04B4D74}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -3693,7 +3615,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3734,12 +3656,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3ECD8AF-CAD0-4505-B2C0-649D20519F35}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3751,7 +3673,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="28" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -3838,12 +3760,144 @@
         <v>600000</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="30">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="32">
+        <v>30000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A86C37-842A-42C0-A5CB-A1729DD4F028}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.21875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="30">
+        <f>StorageCapacity!B3*0.3</f>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="30">
+        <f>StorageCapacity!B4*0.3</f>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="30">
+        <f>StorageCapacity!B5*0.3</f>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="30">
+        <f>StorageCapacity!B6*0.3</f>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="30">
+        <f>StorageCapacity!B7*0.3</f>
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="30">
+        <f>StorageCapacity!B8*0.3</f>
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="30">
+        <f>StorageCapacity!B9*0.3</f>
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="30">
+        <f>StorageCapacity!B10*0.3</f>
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="30">
+        <f>StorageCapacity!B11*0.3</f>
+        <v>180000</v>
+      </c>
+    </row>
     <row r="12" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="27" t="s">
         <v>97</v>
       </c>
       <c r="B12" s="32">
-        <v>600000</v>
+        <f>StorageCapacity!B13*0.3</f>
+        <v>9000000</v>
       </c>
     </row>
   </sheetData>
@@ -3924,135 +3978,11 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A86C37-842A-42C0-A5CB-A1729DD4F028}">
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.6640625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.21875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="30">
-        <f>StorageCapacity!B3*0.3</f>
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="30">
-        <f>StorageCapacity!B4*0.3</f>
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="30">
-        <f>StorageCapacity!B5*0.3</f>
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="30">
-        <f>StorageCapacity!B6*0.3</f>
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="30">
-        <f>StorageCapacity!B7*0.3</f>
-        <v>90000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="30">
-        <f>StorageCapacity!B8*0.3</f>
-        <v>90000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="30">
-        <f>StorageCapacity!B9*0.3</f>
-        <v>90000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="30">
-        <f>StorageCapacity!B10*0.3</f>
-        <v>90000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="30">
-        <f>StorageCapacity!B11*0.3</f>
-        <v>180000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="B12" s="32">
-        <f>StorageCapacity!B12*0.3</f>
-        <v>180000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF01EBE-6835-4B3D-A904-8EE69C83B85A}">
   <dimension ref="A1:Z38"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4064,7 +3994,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -4161,17 +4091,17 @@
         <f>IF(Topology!F3=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="G3" s="7" t="str">
+      <c r="G3" s="7">
         <f>IF(Topology!G3=1,$Z$3,"")</f>
-        <v/>
-      </c>
-      <c r="H3" s="7" t="str">
+        <v>200000</v>
+      </c>
+      <c r="H3" s="7">
         <f>IF(Topology!H3=1,$Z$3,"")</f>
-        <v/>
-      </c>
-      <c r="I3" s="7" t="str">
+        <v>200000</v>
+      </c>
+      <c r="I3" s="7">
         <f>IF(Topology!I3=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="J3" s="7" t="str">
         <f>IF(Topology!J3=1,$Z$3,"")</f>
@@ -4191,11 +4121,11 @@
       </c>
       <c r="N3" s="7">
         <f>IF(Topology!N3=1,$Z$3,"")</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="O3" s="7">
         <f>IF(Topology!O3=1,$Z$3,"")</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="P3" s="7" t="str">
         <f>IF(Topology!P3=1,$Z$3,"")</f>
@@ -4233,7 +4163,7 @@
         <v>99</v>
       </c>
       <c r="Z3" s="6">
-        <v>100000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -4243,9 +4173,9 @@
       <c r="B4" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="7" t="str">
         <f>IF(Topology!C4=1,$Z$3,"")</f>
-        <v>100000</v>
+        <v/>
       </c>
       <c r="D4" s="7" t="str">
         <f>IF(Topology!D4=1,$Z$3,"")</f>
@@ -4259,17 +4189,17 @@
         <f>IF(Topology!F4=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="G4" s="7" t="str">
+      <c r="G4" s="7">
         <f>IF(Topology!G4=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="H4" s="7" t="str">
         <f>IF(Topology!H4=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="I4" s="7" t="str">
+      <c r="I4" s="7">
         <f>IF(Topology!I4=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="J4" s="7" t="str">
         <f>IF(Topology!J4=1,$Z$3,"")</f>
@@ -4277,7 +4207,7 @@
       </c>
       <c r="K4" s="7">
         <f>IF(Topology!K4=1,$Z$3,"")</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="L4" s="7" t="str">
         <f>IF(Topology!L4=1,$Z$3,"")</f>
@@ -4289,7 +4219,7 @@
       </c>
       <c r="N4" s="7">
         <f>IF(Topology!N4=1,$Z$3,"")</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="O4" s="7" t="str">
         <f>IF(Topology!O4=1,$Z$3,"")</f>
@@ -4335,9 +4265,9 @@
       <c r="B5" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="7" t="str">
         <f>IF(Topology!C5=1,$Z$3,"")</f>
-        <v>100000</v>
+        <v/>
       </c>
       <c r="D5" s="7" t="str">
         <f>IF(Topology!D5=1,$Z$3,"")</f>
@@ -4355,9 +4285,9 @@
         <f>IF(Topology!G5=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="H5" s="7" t="str">
+      <c r="H5" s="7">
         <f>IF(Topology!H5=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="I5" s="7" t="str">
         <f>IF(Topology!I5=1,$Z$3,"")</f>
@@ -4401,7 +4331,7 @@
       </c>
       <c r="S5" s="7">
         <f>IF(Topology!S5=1,$Z$3,"")</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="T5" s="7" t="str">
         <f>IF(Topology!T5=1,$Z$3,"")</f>
@@ -4427,9 +4357,9 @@
       <c r="B6" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="7" t="str">
         <f>IF(Topology!C6=1,$Z$3,"")</f>
-        <v>100000</v>
+        <v/>
       </c>
       <c r="D6" s="7" t="str">
         <f>IF(Topology!D6=1,$Z$3,"")</f>
@@ -4455,9 +4385,9 @@
         <f>IF(Topology!I6=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="J6" s="7" t="str">
+      <c r="J6" s="7">
         <f>IF(Topology!J6=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="K6" s="7" t="str">
         <f>IF(Topology!K6=1,$Z$3,"")</f>
@@ -4493,7 +4423,7 @@
       </c>
       <c r="S6" s="7">
         <f>IF(Topology!S6=1,$Z$3,"")</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="T6" s="7" t="str">
         <f>IF(Topology!T6=1,$Z$3,"")</f>
@@ -4551,9 +4481,9 @@
         <f>IF(Topology!J7=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="K7" s="7" t="str">
+      <c r="K7" s="7">
         <f>IF(Topology!K7=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="L7" s="7" t="str">
         <f>IF(Topology!L7=1,$Z$3,"")</f>
@@ -4567,17 +4497,17 @@
         <f>IF(Topology!N7=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="O7" s="7" t="str">
+      <c r="O7" s="7">
         <f>IF(Topology!O7=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="P7" s="7" t="str">
         <f>IF(Topology!P7=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="Q7" s="7" t="str">
+      <c r="Q7" s="7">
         <f>IF(Topology!Q7=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="R7" s="7" t="str">
         <f>IF(Topology!R7=1,$Z$3,"")</f>
@@ -4661,7 +4591,7 @@
       </c>
       <c r="O8" s="7">
         <f>IF(Topology!O8=1,$Z$3,"")</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="P8" s="7" t="str">
         <f>IF(Topology!P8=1,$Z$3,"")</f>
@@ -4747,9 +4677,9 @@
         <f>IF(Topology!M9=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="N9" s="7" t="str">
+      <c r="N9" s="7">
         <f>IF(Topology!N9=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="O9" s="7" t="str">
         <f>IF(Topology!O9=1,$Z$3,"")</f>
@@ -4831,9 +4761,9 @@
         <f>IF(Topology!K10=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="L10" s="7" t="str">
+      <c r="L10" s="7">
         <f>IF(Topology!L10=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="M10" s="7" t="str">
         <f>IF(Topology!M10=1,$Z$3,"")</f>
@@ -4859,9 +4789,9 @@
         <f>IF(Topology!R10=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="S10" s="7" t="str">
+      <c r="S10" s="7">
         <f>IF(Topology!S10=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="T10" s="7" t="str">
         <f>IF(Topology!T10=1,$Z$3,"")</f>
@@ -4903,9 +4833,9 @@
         <f>IF(Topology!F11=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="G11" s="7" t="str">
+      <c r="G11" s="7">
         <f>IF(Topology!G11=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="H11" s="7" t="str">
         <f>IF(Topology!H11=1,$Z$3,"")</f>
@@ -4931,9 +4861,9 @@
         <f>IF(Topology!M11=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="N11" s="7" t="str">
+      <c r="N11" s="7">
         <f>IF(Topology!N11=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="O11" s="7" t="str">
         <f>IF(Topology!O11=1,$Z$3,"")</f>
@@ -4947,9 +4877,9 @@
         <f>IF(Topology!Q11=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="R11" s="7" t="str">
+      <c r="R11" s="7">
         <f>IF(Topology!R11=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="S11" s="7" t="str">
         <f>IF(Topology!S11=1,$Z$3,"")</f>
@@ -5007,9 +4937,9 @@
         <f>IF(Topology!I12=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="J12" s="7" t="str">
+      <c r="J12" s="7">
         <f>IF(Topology!J12=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="K12" s="7" t="str">
         <f>IF(Topology!K12=1,$Z$3,"")</f>
@@ -5031,17 +4961,17 @@
         <f>IF(Topology!O12=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="P12" s="7" t="str">
+      <c r="P12" s="7">
         <f>IF(Topology!P12=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="Q12" s="7" t="str">
         <f>IF(Topology!Q12=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="R12" s="7" t="str">
+      <c r="R12" s="7">
         <f>IF(Topology!R12=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="S12" s="7" t="str">
         <f>IF(Topology!S12=1,$Z$3,"")</f>
@@ -5071,21 +5001,21 @@
       <c r="B13" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="7" t="str">
+      <c r="C13" s="7">
         <f>IF(Topology!C13=1,$Z$3,"")</f>
-        <v/>
-      </c>
-      <c r="D13" s="7" t="str">
+        <v>200000</v>
+      </c>
+      <c r="D13" s="7">
         <f>IF(Topology!D13=1,$Z$3,"")</f>
-        <v/>
-      </c>
-      <c r="E13" s="7" t="str">
+        <v>200000</v>
+      </c>
+      <c r="E13" s="7">
         <f>IF(Topology!E13=1,$Z$3,"")</f>
-        <v/>
-      </c>
-      <c r="F13" s="7" t="str">
+        <v>200000</v>
+      </c>
+      <c r="F13" s="7">
         <f>IF(Topology!F13=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="G13" s="7" t="str">
         <f>IF(Topology!G13=1,$Z$3,"")</f>
@@ -5187,17 +5117,17 @@
         <f>IF(Topology!H14=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="I14" s="7" t="str">
+      <c r="I14" s="7">
         <f>IF(Topology!I14=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="J14" s="7" t="str">
         <f>IF(Topology!J14=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="K14" s="7" t="str">
+      <c r="K14" s="7">
         <f>IF(Topology!K14=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="L14" s="7" t="str">
         <f>IF(Topology!L14=1,$Z$3,"")</f>
@@ -5271,13 +5201,13 @@
         <f>IF(Topology!F15=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="G15" s="7" t="str">
+      <c r="G15" s="7">
         <f>IF(Topology!G15=1,$Z$3,"")</f>
-        <v/>
-      </c>
-      <c r="H15" s="7" t="str">
+        <v>200000</v>
+      </c>
+      <c r="H15" s="7">
         <f>IF(Topology!H15=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="I15" s="7" t="str">
         <f>IF(Topology!I15=1,$Z$3,"")</f>
@@ -5307,9 +5237,9 @@
         <f>IF(Topology!O15=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="P15" s="7" t="str">
+      <c r="P15" s="7">
         <f>IF(Topology!P15=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="Q15" s="7" t="str">
         <f>IF(Topology!Q15=1,$Z$3,"")</f>
@@ -5383,9 +5313,9 @@
         <f>IF(Topology!K16=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="L16" s="7" t="str">
+      <c r="L16" s="7">
         <f>IF(Topology!L16=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="M16" s="7" t="str">
         <f>IF(Topology!M16=1,$Z$3,"")</f>
@@ -5395,17 +5325,17 @@
         <f>IF(Topology!N16=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="O16" s="7" t="str">
+      <c r="O16" s="7">
         <f>IF(Topology!O16=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="P16" s="7" t="str">
         <f>IF(Topology!P16=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="Q16" s="7" t="str">
+      <c r="Q16" s="7">
         <f>IF(Topology!Q16=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="R16" s="7" t="str">
         <f>IF(Topology!R16=1,$Z$3,"")</f>
@@ -5455,9 +5385,9 @@
         <f>IF(Topology!F17=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="G17" s="7" t="str">
+      <c r="G17" s="7">
         <f>IF(Topology!G17=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="H17" s="7" t="str">
         <f>IF(Topology!H17=1,$Z$3,"")</f>
@@ -5491,17 +5421,17 @@
         <f>IF(Topology!O17=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="P17" s="7" t="str">
+      <c r="P17" s="7">
         <f>IF(Topology!P17=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="Q17" s="7" t="str">
         <f>IF(Topology!Q17=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="R17" s="7" t="str">
+      <c r="R17" s="7">
         <f>IF(Topology!R17=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="S17" s="7" t="str">
         <f>IF(Topology!S17=1,$Z$3,"")</f>
@@ -5563,13 +5493,13 @@
         <f>IF(Topology!J18=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="K18" s="7" t="str">
+      <c r="K18" s="7">
         <f>IF(Topology!K18=1,$Z$3,"")</f>
-        <v/>
-      </c>
-      <c r="L18" s="7" t="str">
+        <v>200000</v>
+      </c>
+      <c r="L18" s="7">
         <f>IF(Topology!L18=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="M18" s="7" t="str">
         <f>IF(Topology!M18=1,$Z$3,"")</f>
@@ -5587,9 +5517,9 @@
         <f>IF(Topology!P18=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="Q18" s="7" t="str">
+      <c r="Q18" s="7">
         <f>IF(Topology!Q18=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="R18" s="7" t="str">
         <f>IF(Topology!R18=1,$Z$3,"")</f>
@@ -5599,9 +5529,9 @@
         <f>IF(Topology!S18=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="T18" s="7" t="str">
+      <c r="T18" s="7">
         <f>IF(Topology!T18=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="U18" s="7" t="str">
         <f>IF(Topology!U18=1,$Z$3,"")</f>
@@ -5651,17 +5581,17 @@
         <f>IF(Topology!I19=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="J19" s="7" t="str">
+      <c r="J19" s="7">
         <f>IF(Topology!J19=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="K19" s="7" t="str">
         <f>IF(Topology!K19=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="L19" s="7" t="str">
+      <c r="L19" s="7">
         <f>IF(Topology!L19=1,$Z$3,"")</f>
-        <v/>
+        <v>200000</v>
       </c>
       <c r="M19" s="7" t="str">
         <f>IF(Topology!M19=1,$Z$3,"")</f>
@@ -5825,19 +5755,19 @@
       </c>
       <c r="G21" s="7">
         <f>IF(Topology!G21=1,$Z$3,"")</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="H21" s="7">
         <f>IF(Topology!H21=1,$Z$3,"")</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="I21" s="7">
         <f>IF(Topology!I21=1,$Z$3,"")</f>
-        <v>100000</v>
-      </c>
-      <c r="J21" s="7">
+        <v>200000</v>
+      </c>
+      <c r="J21" s="7" t="str">
         <f>IF(Topology!J21=1,$Z$3,"")</f>
-        <v>100000</v>
+        <v/>
       </c>
       <c r="K21" s="7" t="str">
         <f>IF(Topology!K21=1,$Z$3,"")</f>
@@ -5915,21 +5845,21 @@
         <f>IF(Topology!F22=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="7" t="str">
         <f>IF(Topology!G22=1,$Z$3,"")</f>
-        <v>100000</v>
+        <v/>
       </c>
       <c r="H22" s="7">
         <f>IF(Topology!H22=1,$Z$3,"")</f>
-        <v>100000</v>
-      </c>
-      <c r="I22" s="7">
+        <v>200000</v>
+      </c>
+      <c r="I22" s="7" t="str">
         <f>IF(Topology!I22=1,$Z$3,"")</f>
-        <v>100000</v>
-      </c>
-      <c r="J22" s="7">
+        <v/>
+      </c>
+      <c r="J22" s="7" t="str">
         <f>IF(Topology!J22=1,$Z$3,"")</f>
-        <v>100000</v>
+        <v/>
       </c>
       <c r="K22" s="7" t="str">
         <f>IF(Topology!K22=1,$Z$3,"")</f>
@@ -6007,21 +5937,21 @@
         <f>IF(Topology!F23=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="8" t="str">
         <f>IF(Topology!G23=1,$Z$3,"")</f>
-        <v>100000</v>
-      </c>
-      <c r="H23" s="8">
+        <v/>
+      </c>
+      <c r="H23" s="8" t="str">
         <f>IF(Topology!H23=1,$Z$3,"")</f>
-        <v>100000</v>
-      </c>
-      <c r="I23" s="8">
+        <v/>
+      </c>
+      <c r="I23" s="8" t="str">
         <f>IF(Topology!I23=1,$Z$3,"")</f>
-        <v>100000</v>
+        <v/>
       </c>
       <c r="J23" s="8">
         <f>IF(Topology!J23=1,$Z$3,"")</f>
-        <v>100000</v>
+        <v>200000</v>
       </c>
       <c r="K23" s="8" t="str">
         <f>IF(Topology!K23=1,$Z$3,"")</f>
@@ -6125,7 +6055,7 @@
       </c>
       <c r="M24" s="7">
         <f>IF(Topology!M24=1,$Z$24,"")</f>
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="N24" s="7" t="str">
         <f>IF(Topology!N24=1,$Z$24,"")</f>
@@ -6171,7 +6101,7 @@
         <v>100</v>
       </c>
       <c r="Z24" s="1">
-        <v>50000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.3">
@@ -6223,7 +6153,7 @@
       </c>
       <c r="M25" s="7">
         <f>IF(Topology!M25=1,$Z$24,"")</f>
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="N25" s="7" t="str">
         <f>IF(Topology!N25=1,$Z$24,"")</f>
@@ -6315,7 +6245,7 @@
       </c>
       <c r="M26" s="7">
         <f>IF(Topology!M26=1,$Z$24,"")</f>
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="N26" s="7" t="str">
         <f>IF(Topology!N26=1,$Z$24,"")</f>
@@ -6407,7 +6337,7 @@
       </c>
       <c r="M27" s="7">
         <f>IF(Topology!M27=1,$Z$24,"")</f>
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="N27" s="7" t="str">
         <f>IF(Topology!N27=1,$Z$24,"")</f>
@@ -6457,9 +6387,9 @@
       <c r="B28" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="7" t="str">
         <f>IF(Topology!C28=1,$Z$24,"")</f>
-        <v>50000</v>
+        <v/>
       </c>
       <c r="D28" s="7" t="str">
         <f>IF(Topology!D28=1,$Z$24,"")</f>
@@ -6499,7 +6429,7 @@
       </c>
       <c r="M28" s="7">
         <f>IF(Topology!M28=1,$Z$24,"")</f>
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="N28" s="7" t="str">
         <f>IF(Topology!N28=1,$Z$24,"")</f>
@@ -6549,9 +6479,9 @@
       <c r="B29" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="7" t="str">
         <f>IF(Topology!C29=1,$Z$24,"")</f>
-        <v>50000</v>
+        <v/>
       </c>
       <c r="D29" s="7" t="str">
         <f>IF(Topology!D29=1,$Z$24,"")</f>
@@ -6591,7 +6521,7 @@
       </c>
       <c r="M29" s="7">
         <f>IF(Topology!M29=1,$Z$24,"")</f>
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="N29" s="7" t="str">
         <f>IF(Topology!N29=1,$Z$24,"")</f>
@@ -6641,9 +6571,9 @@
       <c r="B30" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="7" t="str">
         <f>IF(Topology!C30=1,$Z$24,"")</f>
-        <v>50000</v>
+        <v/>
       </c>
       <c r="D30" s="7" t="str">
         <f>IF(Topology!D30=1,$Z$24,"")</f>
@@ -6683,7 +6613,7 @@
       </c>
       <c r="M30" s="7">
         <f>IF(Topology!M30=1,$Z$24,"")</f>
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="N30" s="7" t="str">
         <f>IF(Topology!N30=1,$Z$24,"")</f>
@@ -6733,9 +6663,9 @@
       <c r="B31" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="7" t="str">
         <f>IF(Topology!C31=1,$Z$24,"")</f>
-        <v>50000</v>
+        <v/>
       </c>
       <c r="D31" s="7" t="str">
         <f>IF(Topology!D31=1,$Z$24,"")</f>
@@ -6775,7 +6705,7 @@
       </c>
       <c r="M31" s="7">
         <f>IF(Topology!M31=1,$Z$24,"")</f>
-        <v>50000</v>
+        <v>100000</v>
       </c>
       <c r="N31" s="7" t="str">
         <f>IF(Topology!N31=1,$Z$24,"")</f>
@@ -7209,21 +7139,21 @@
         <f>IF(Topology!F36=1,$Z$24,"")</f>
         <v/>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="7" t="str">
         <f>IF(Topology!G36=1,$Z$24,"")</f>
-        <v>50000</v>
-      </c>
-      <c r="H36" s="7">
+        <v/>
+      </c>
+      <c r="H36" s="7" t="str">
         <f>IF(Topology!H36=1,$Z$24,"")</f>
-        <v>50000</v>
-      </c>
-      <c r="I36" s="7">
+        <v/>
+      </c>
+      <c r="I36" s="7" t="str">
         <f>IF(Topology!I36=1,$Z$24,"")</f>
-        <v>50000</v>
-      </c>
-      <c r="J36" s="7">
+        <v/>
+      </c>
+      <c r="J36" s="7" t="str">
         <f>IF(Topology!J36=1,$Z$24,"")</f>
-        <v>50000</v>
+        <v/>
       </c>
       <c r="K36" s="7" t="str">
         <f>IF(Topology!K36=1,$Z$24,"")</f>
@@ -7301,21 +7231,21 @@
         <f>IF(Topology!F37=1,$Z$24,"")</f>
         <v/>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="7" t="str">
         <f>IF(Topology!G37=1,$Z$24,"")</f>
-        <v>50000</v>
-      </c>
-      <c r="H37" s="7">
+        <v/>
+      </c>
+      <c r="H37" s="7" t="str">
         <f>IF(Topology!H37=1,$Z$24,"")</f>
-        <v>50000</v>
-      </c>
-      <c r="I37" s="7">
+        <v/>
+      </c>
+      <c r="I37" s="7" t="str">
         <f>IF(Topology!I37=1,$Z$24,"")</f>
-        <v>50000</v>
-      </c>
-      <c r="J37" s="7">
+        <v/>
+      </c>
+      <c r="J37" s="7" t="str">
         <f>IF(Topology!J37=1,$Z$24,"")</f>
-        <v>50000</v>
+        <v/>
       </c>
       <c r="K37" s="7" t="str">
         <f>IF(Topology!K37=1,$Z$24,"")</f>
@@ -7393,21 +7323,21 @@
         <f>IF(Topology!F38=1,$Z$24,"")</f>
         <v/>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="8" t="str">
         <f>IF(Topology!G38=1,$Z$24,"")</f>
-        <v>50000</v>
-      </c>
-      <c r="H38" s="8">
+        <v/>
+      </c>
+      <c r="H38" s="8" t="str">
         <f>IF(Topology!H38=1,$Z$24,"")</f>
-        <v>50000</v>
-      </c>
-      <c r="I38" s="8">
+        <v/>
+      </c>
+      <c r="I38" s="8" t="str">
         <f>IF(Topology!I38=1,$Z$24,"")</f>
-        <v>50000</v>
-      </c>
-      <c r="J38" s="8">
+        <v/>
+      </c>
+      <c r="J38" s="8" t="str">
         <f>IF(Topology!J38=1,$Z$24,"")</f>
-        <v>50000</v>
+        <v/>
       </c>
       <c r="K38" s="8" t="str">
         <f>IF(Topology!K38=1,$Z$24,"")</f>
@@ -7468,7 +7398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F58DBFDB-DAAF-4E8D-87E8-D26A8499FEF7}">
   <dimension ref="A1:Z38"/>
   <sheetViews>
@@ -7487,7 +7417,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -7584,17 +7514,17 @@
         <f>IF(Topology!F3=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="G3" s="7" t="str">
+      <c r="G3" s="7">
         <f>IF(Topology!G3=1,$Z$3,"")</f>
-        <v/>
-      </c>
-      <c r="H3" s="7" t="str">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="H3" s="7">
         <f>IF(Topology!H3=1,$Z$3,"")</f>
-        <v/>
-      </c>
-      <c r="I3" s="7" t="str">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I3" s="7">
         <f>IF(Topology!I3=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="J3" s="7" t="str">
         <f>IF(Topology!J3=1,$Z$3,"")</f>
@@ -7653,7 +7583,7 @@
         <v/>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Z3" s="6">
         <f>0.0001/10</f>
@@ -7667,9 +7597,9 @@
       <c r="B4" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="7" t="str">
         <f>IF(Topology!C4=1,$Z$3,"")</f>
-        <v>1.0000000000000001E-5</v>
+        <v/>
       </c>
       <c r="D4" s="7" t="str">
         <f>IF(Topology!D4=1,$Z$3,"")</f>
@@ -7683,17 +7613,17 @@
         <f>IF(Topology!F4=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="G4" s="7" t="str">
+      <c r="G4" s="7">
         <f>IF(Topology!G4=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="H4" s="7" t="str">
         <f>IF(Topology!H4=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="I4" s="7" t="str">
+      <c r="I4" s="7">
         <f>IF(Topology!I4=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="J4" s="7" t="str">
         <f>IF(Topology!J4=1,$Z$3,"")</f>
@@ -7759,9 +7689,9 @@
       <c r="B5" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="7" t="str">
         <f>IF(Topology!C5=1,$Z$3,"")</f>
-        <v>1.0000000000000001E-5</v>
+        <v/>
       </c>
       <c r="D5" s="7" t="str">
         <f>IF(Topology!D5=1,$Z$3,"")</f>
@@ -7779,9 +7709,9 @@
         <f>IF(Topology!G5=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="H5" s="7" t="str">
+      <c r="H5" s="7">
         <f>IF(Topology!H5=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="I5" s="7" t="str">
         <f>IF(Topology!I5=1,$Z$3,"")</f>
@@ -7851,9 +7781,9 @@
       <c r="B6" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="7" t="str">
         <f>IF(Topology!C6=1,$Z$3,"")</f>
-        <v>1.0000000000000001E-5</v>
+        <v/>
       </c>
       <c r="D6" s="7" t="str">
         <f>IF(Topology!D6=1,$Z$3,"")</f>
@@ -7879,9 +7809,9 @@
         <f>IF(Topology!I6=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="J6" s="7" t="str">
+      <c r="J6" s="7">
         <f>IF(Topology!J6=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K6" s="7" t="str">
         <f>IF(Topology!K6=1,$Z$3,"")</f>
@@ -7975,9 +7905,9 @@
         <f>IF(Topology!J7=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="K7" s="7" t="str">
+      <c r="K7" s="7">
         <f>IF(Topology!K7=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="L7" s="7" t="str">
         <f>IF(Topology!L7=1,$Z$3,"")</f>
@@ -7991,17 +7921,17 @@
         <f>IF(Topology!N7=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="O7" s="7" t="str">
+      <c r="O7" s="7">
         <f>IF(Topology!O7=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="P7" s="7" t="str">
         <f>IF(Topology!P7=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="Q7" s="7" t="str">
+      <c r="Q7" s="7">
         <f>IF(Topology!Q7=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="R7" s="7" t="str">
         <f>IF(Topology!R7=1,$Z$3,"")</f>
@@ -8171,9 +8101,9 @@
         <f>IF(Topology!M9=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="N9" s="7" t="str">
+      <c r="N9" s="7">
         <f>IF(Topology!N9=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="O9" s="7" t="str">
         <f>IF(Topology!O9=1,$Z$3,"")</f>
@@ -8255,9 +8185,9 @@
         <f>IF(Topology!K10=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="L10" s="7" t="str">
+      <c r="L10" s="7">
         <f>IF(Topology!L10=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="M10" s="7" t="str">
         <f>IF(Topology!M10=1,$Z$3,"")</f>
@@ -8283,9 +8213,9 @@
         <f>IF(Topology!R10=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="S10" s="7" t="str">
+      <c r="S10" s="7">
         <f>IF(Topology!S10=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="T10" s="7" t="str">
         <f>IF(Topology!T10=1,$Z$3,"")</f>
@@ -8327,9 +8257,9 @@
         <f>IF(Topology!F11=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="G11" s="7" t="str">
+      <c r="G11" s="7">
         <f>IF(Topology!G11=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="H11" s="7" t="str">
         <f>IF(Topology!H11=1,$Z$3,"")</f>
@@ -8355,9 +8285,9 @@
         <f>IF(Topology!M11=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="N11" s="7" t="str">
+      <c r="N11" s="7">
         <f>IF(Topology!N11=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="O11" s="7" t="str">
         <f>IF(Topology!O11=1,$Z$3,"")</f>
@@ -8371,9 +8301,9 @@
         <f>IF(Topology!Q11=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="R11" s="7" t="str">
+      <c r="R11" s="7">
         <f>IF(Topology!R11=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="S11" s="7" t="str">
         <f>IF(Topology!S11=1,$Z$3,"")</f>
@@ -8431,9 +8361,9 @@
         <f>IF(Topology!I12=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="J12" s="7" t="str">
+      <c r="J12" s="7">
         <f>IF(Topology!J12=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K12" s="7" t="str">
         <f>IF(Topology!K12=1,$Z$3,"")</f>
@@ -8455,17 +8385,17 @@
         <f>IF(Topology!O12=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="P12" s="7" t="str">
+      <c r="P12" s="7">
         <f>IF(Topology!P12=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="Q12" s="7" t="str">
         <f>IF(Topology!Q12=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="R12" s="7" t="str">
+      <c r="R12" s="7">
         <f>IF(Topology!R12=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="S12" s="7" t="str">
         <f>IF(Topology!S12=1,$Z$3,"")</f>
@@ -8495,21 +8425,21 @@
       <c r="B13" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="7" t="str">
+      <c r="C13" s="7">
         <f>IF(Topology!C13=1,$Z$3,"")</f>
-        <v/>
-      </c>
-      <c r="D13" s="7" t="str">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="D13" s="7">
         <f>IF(Topology!D13=1,$Z$3,"")</f>
-        <v/>
-      </c>
-      <c r="E13" s="7" t="str">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E13" s="7">
         <f>IF(Topology!E13=1,$Z$3,"")</f>
-        <v/>
-      </c>
-      <c r="F13" s="7" t="str">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F13" s="7">
         <f>IF(Topology!F13=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="G13" s="7" t="str">
         <f>IF(Topology!G13=1,$Z$3,"")</f>
@@ -8611,17 +8541,17 @@
         <f>IF(Topology!H14=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="I14" s="7" t="str">
+      <c r="I14" s="7">
         <f>IF(Topology!I14=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="J14" s="7" t="str">
         <f>IF(Topology!J14=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="K14" s="7" t="str">
+      <c r="K14" s="7">
         <f>IF(Topology!K14=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="L14" s="7" t="str">
         <f>IF(Topology!L14=1,$Z$3,"")</f>
@@ -8695,13 +8625,13 @@
         <f>IF(Topology!F15=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="G15" s="7" t="str">
+      <c r="G15" s="7">
         <f>IF(Topology!G15=1,$Z$3,"")</f>
-        <v/>
-      </c>
-      <c r="H15" s="7" t="str">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="H15" s="7">
         <f>IF(Topology!H15=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="I15" s="7" t="str">
         <f>IF(Topology!I15=1,$Z$3,"")</f>
@@ -8731,9 +8661,9 @@
         <f>IF(Topology!O15=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="P15" s="7" t="str">
+      <c r="P15" s="7">
         <f>IF(Topology!P15=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="Q15" s="7" t="str">
         <f>IF(Topology!Q15=1,$Z$3,"")</f>
@@ -8807,9 +8737,9 @@
         <f>IF(Topology!K16=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="L16" s="7" t="str">
+      <c r="L16" s="7">
         <f>IF(Topology!L16=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="M16" s="7" t="str">
         <f>IF(Topology!M16=1,$Z$3,"")</f>
@@ -8819,17 +8749,17 @@
         <f>IF(Topology!N16=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="O16" s="7" t="str">
+      <c r="O16" s="7">
         <f>IF(Topology!O16=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="P16" s="7" t="str">
         <f>IF(Topology!P16=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="Q16" s="7" t="str">
+      <c r="Q16" s="7">
         <f>IF(Topology!Q16=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="R16" s="7" t="str">
         <f>IF(Topology!R16=1,$Z$3,"")</f>
@@ -8879,9 +8809,9 @@
         <f>IF(Topology!F17=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="G17" s="7" t="str">
+      <c r="G17" s="7">
         <f>IF(Topology!G17=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="H17" s="7" t="str">
         <f>IF(Topology!H17=1,$Z$3,"")</f>
@@ -8915,17 +8845,17 @@
         <f>IF(Topology!O17=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="P17" s="7" t="str">
+      <c r="P17" s="7">
         <f>IF(Topology!P17=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="Q17" s="7" t="str">
         <f>IF(Topology!Q17=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="R17" s="7" t="str">
+      <c r="R17" s="7">
         <f>IF(Topology!R17=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="S17" s="7" t="str">
         <f>IF(Topology!S17=1,$Z$3,"")</f>
@@ -8987,13 +8917,13 @@
         <f>IF(Topology!J18=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="K18" s="7" t="str">
+      <c r="K18" s="7">
         <f>IF(Topology!K18=1,$Z$3,"")</f>
-        <v/>
-      </c>
-      <c r="L18" s="7" t="str">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="L18" s="7">
         <f>IF(Topology!L18=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="M18" s="7" t="str">
         <f>IF(Topology!M18=1,$Z$3,"")</f>
@@ -9011,9 +8941,9 @@
         <f>IF(Topology!P18=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="Q18" s="7" t="str">
+      <c r="Q18" s="7">
         <f>IF(Topology!Q18=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="R18" s="7" t="str">
         <f>IF(Topology!R18=1,$Z$3,"")</f>
@@ -9023,9 +8953,9 @@
         <f>IF(Topology!S18=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="T18" s="7" t="str">
+      <c r="T18" s="7">
         <f>IF(Topology!T18=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="U18" s="7" t="str">
         <f>IF(Topology!U18=1,$Z$3,"")</f>
@@ -9075,17 +9005,17 @@
         <f>IF(Topology!I19=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="J19" s="7" t="str">
+      <c r="J19" s="7">
         <f>IF(Topology!J19=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="K19" s="7" t="str">
         <f>IF(Topology!K19=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="L19" s="7" t="str">
+      <c r="L19" s="7">
         <f>IF(Topology!L19=1,$Z$3,"")</f>
-        <v/>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="M19" s="7" t="str">
         <f>IF(Topology!M19=1,$Z$3,"")</f>
@@ -9259,9 +9189,9 @@
         <f>IF(Topology!I21=1,$Z$3,"")</f>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="7" t="str">
         <f>IF(Topology!J21=1,$Z$3,"")</f>
-        <v>1.0000000000000001E-5</v>
+        <v/>
       </c>
       <c r="K21" s="7" t="str">
         <f>IF(Topology!K21=1,$Z$3,"")</f>
@@ -9339,21 +9269,21 @@
         <f>IF(Topology!F22=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="7" t="str">
         <f>IF(Topology!G22=1,$Z$3,"")</f>
-        <v>1.0000000000000001E-5</v>
+        <v/>
       </c>
       <c r="H22" s="7">
         <f>IF(Topology!H22=1,$Z$3,"")</f>
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="7" t="str">
         <f>IF(Topology!I22=1,$Z$3,"")</f>
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="J22" s="7">
+        <v/>
+      </c>
+      <c r="J22" s="7" t="str">
         <f>IF(Topology!J22=1,$Z$3,"")</f>
-        <v>1.0000000000000001E-5</v>
+        <v/>
       </c>
       <c r="K22" s="7" t="str">
         <f>IF(Topology!K22=1,$Z$3,"")</f>
@@ -9431,17 +9361,17 @@
         <f>IF(Topology!F23=1,$Z$3,"")</f>
         <v/>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="8" t="str">
         <f>IF(Topology!G23=1,$Z$3,"")</f>
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="H23" s="8">
+        <v/>
+      </c>
+      <c r="H23" s="8" t="str">
         <f>IF(Topology!H23=1,$Z$3,"")</f>
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="I23" s="8">
+        <v/>
+      </c>
+      <c r="I23" s="8" t="str">
         <f>IF(Topology!I23=1,$Z$3,"")</f>
-        <v>1.0000000000000001E-5</v>
+        <v/>
       </c>
       <c r="J23" s="8">
         <f>IF(Topology!J23=1,$Z$3,"")</f>
@@ -9592,7 +9522,7 @@
         <v/>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Z24" s="1">
         <f>100/(100*15)</f>
@@ -9882,9 +9812,9 @@
       <c r="B28" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="7" t="str">
         <f>IF(Topology!C28=1,$Z$24,"")</f>
-        <v>6.6666666666666666E-2</v>
+        <v/>
       </c>
       <c r="D28" s="7" t="str">
         <f>IF(Topology!D28=1,$Z$24,"")</f>
@@ -9974,9 +9904,9 @@
       <c r="B29" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="7" t="str">
         <f>IF(Topology!C29=1,$Z$24,"")</f>
-        <v>6.6666666666666666E-2</v>
+        <v/>
       </c>
       <c r="D29" s="7" t="str">
         <f>IF(Topology!D29=1,$Z$24,"")</f>
@@ -10066,9 +9996,9 @@
       <c r="B30" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="7" t="str">
         <f>IF(Topology!C30=1,$Z$24,"")</f>
-        <v>6.6666666666666666E-2</v>
+        <v/>
       </c>
       <c r="D30" s="7" t="str">
         <f>IF(Topology!D30=1,$Z$24,"")</f>
@@ -10158,9 +10088,9 @@
       <c r="B31" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="7" t="str">
         <f>IF(Topology!C31=1,$Z$24,"")</f>
-        <v>6.6666666666666666E-2</v>
+        <v/>
       </c>
       <c r="D31" s="7" t="str">
         <f>IF(Topology!D31=1,$Z$24,"")</f>
@@ -10634,21 +10564,21 @@
         <f>IF(Topology!F36=1,$Z$24,"")</f>
         <v/>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="7" t="str">
         <f>IF(Topology!G36=1,$Z$24,"")</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="H36" s="7">
+        <v/>
+      </c>
+      <c r="H36" s="7" t="str">
         <f>IF(Topology!H36=1,$Z$24,"")</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="I36" s="7">
+        <v/>
+      </c>
+      <c r="I36" s="7" t="str">
         <f>IF(Topology!I36=1,$Z$24,"")</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="J36" s="7">
+        <v/>
+      </c>
+      <c r="J36" s="7" t="str">
         <f>IF(Topology!J36=1,$Z$24,"")</f>
-        <v>6.6666666666666666E-2</v>
+        <v/>
       </c>
       <c r="K36" s="7" t="str">
         <f>IF(Topology!K36=1,$Z$24,"")</f>
@@ -10726,21 +10656,21 @@
         <f>IF(Topology!F37=1,$Z$24,"")</f>
         <v/>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="7" t="str">
         <f>IF(Topology!G37=1,$Z$24,"")</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="H37" s="7">
+        <v/>
+      </c>
+      <c r="H37" s="7" t="str">
         <f>IF(Topology!H37=1,$Z$24,"")</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="I37" s="7">
+        <v/>
+      </c>
+      <c r="I37" s="7" t="str">
         <f>IF(Topology!I37=1,$Z$24,"")</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="J37" s="7">
+        <v/>
+      </c>
+      <c r="J37" s="7" t="str">
         <f>IF(Topology!J37=1,$Z$24,"")</f>
-        <v>6.6666666666666666E-2</v>
+        <v/>
       </c>
       <c r="K37" s="7" t="str">
         <f>IF(Topology!K37=1,$Z$24,"")</f>
@@ -10818,21 +10748,21 @@
         <f>IF(Topology!F38=1,$Z$24,"")</f>
         <v/>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="8" t="str">
         <f>IF(Topology!G38=1,$Z$24,"")</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="H38" s="8">
+        <v/>
+      </c>
+      <c r="H38" s="8" t="str">
         <f>IF(Topology!H38=1,$Z$24,"")</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="I38" s="8">
+        <v/>
+      </c>
+      <c r="I38" s="8" t="str">
         <f>IF(Topology!I38=1,$Z$24,"")</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="J38" s="8">
+        <v/>
+      </c>
+      <c r="J38" s="8" t="str">
         <f>IF(Topology!J38=1,$Z$24,"")</f>
-        <v>6.6666666666666666E-2</v>
+        <v/>
       </c>
       <c r="K38" s="8" t="str">
         <f>IF(Topology!K38=1,$Z$24,"")</f>
@@ -10893,11 +10823,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9EA953B-B199-4B9E-AD42-E5A4D6CF7D32}">
   <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
@@ -10910,7 +10840,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -11007,17 +10937,17 @@
         <f>IF(Topology!F3=1,10,"")</f>
         <v/>
       </c>
-      <c r="G3" s="7" t="str">
+      <c r="G3" s="7">
         <f>IF(Topology!G3=1,10,"")</f>
-        <v/>
-      </c>
-      <c r="H3" s="7" t="str">
+        <v>10</v>
+      </c>
+      <c r="H3" s="7">
         <f>IF(Topology!H3=1,10,"")</f>
-        <v/>
-      </c>
-      <c r="I3" s="7" t="str">
+        <v>10</v>
+      </c>
+      <c r="I3" s="7">
         <f>IF(Topology!I3=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="J3" s="7" t="str">
         <f>IF(Topology!J3=1,10,"")</f>
@@ -11083,9 +11013,9 @@
       <c r="B4" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="7" t="str">
         <f>IF(Topology!C4=1,10,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="D4" s="7" t="str">
         <f>IF(Topology!D4=1,10,"")</f>
@@ -11099,17 +11029,17 @@
         <f>IF(Topology!F4=1,10,"")</f>
         <v/>
       </c>
-      <c r="G4" s="7" t="str">
+      <c r="G4" s="7">
         <f>IF(Topology!G4=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="H4" s="7" t="str">
         <f>IF(Topology!H4=1,10,"")</f>
         <v/>
       </c>
-      <c r="I4" s="7" t="str">
+      <c r="I4" s="7">
         <f>IF(Topology!I4=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="J4" s="7" t="str">
         <f>IF(Topology!J4=1,10,"")</f>
@@ -11175,9 +11105,9 @@
       <c r="B5" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="7" t="str">
         <f>IF(Topology!C5=1,10,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="D5" s="7" t="str">
         <f>IF(Topology!D5=1,10,"")</f>
@@ -11195,9 +11125,9 @@
         <f>IF(Topology!G5=1,10,"")</f>
         <v/>
       </c>
-      <c r="H5" s="7" t="str">
+      <c r="H5" s="7">
         <f>IF(Topology!H5=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="I5" s="7" t="str">
         <f>IF(Topology!I5=1,10,"")</f>
@@ -11267,9 +11197,9 @@
       <c r="B6" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="7" t="str">
         <f>IF(Topology!C6=1,10,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="D6" s="7" t="str">
         <f>IF(Topology!D6=1,10,"")</f>
@@ -11295,9 +11225,9 @@
         <f>IF(Topology!I6=1,10,"")</f>
         <v/>
       </c>
-      <c r="J6" s="7" t="str">
+      <c r="J6" s="7">
         <f>IF(Topology!J6=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="K6" s="7" t="str">
         <f>IF(Topology!K6=1,10,"")</f>
@@ -11391,9 +11321,9 @@
         <f>IF(Topology!J7=1,10,"")</f>
         <v/>
       </c>
-      <c r="K7" s="7" t="str">
+      <c r="K7" s="7">
         <f>IF(Topology!K7=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="L7" s="7" t="str">
         <f>IF(Topology!L7=1,10,"")</f>
@@ -11407,17 +11337,17 @@
         <f>IF(Topology!N7=1,10,"")</f>
         <v/>
       </c>
-      <c r="O7" s="7" t="str">
+      <c r="O7" s="7">
         <f>IF(Topology!O7=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="P7" s="7" t="str">
         <f>IF(Topology!P7=1,10,"")</f>
         <v/>
       </c>
-      <c r="Q7" s="7" t="str">
+      <c r="Q7" s="7">
         <f>IF(Topology!Q7=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="R7" s="7" t="str">
         <f>IF(Topology!R7=1,10,"")</f>
@@ -11587,9 +11517,9 @@
         <f>IF(Topology!M9=1,10,"")</f>
         <v/>
       </c>
-      <c r="N9" s="7" t="str">
+      <c r="N9" s="7">
         <f>IF(Topology!N9=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="O9" s="7" t="str">
         <f>IF(Topology!O9=1,10,"")</f>
@@ -11671,9 +11601,9 @@
         <f>IF(Topology!K10=1,10,"")</f>
         <v/>
       </c>
-      <c r="L10" s="7" t="str">
+      <c r="L10" s="7">
         <f>IF(Topology!L10=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="M10" s="7" t="str">
         <f>IF(Topology!M10=1,10,"")</f>
@@ -11699,9 +11629,9 @@
         <f>IF(Topology!R10=1,10,"")</f>
         <v/>
       </c>
-      <c r="S10" s="7" t="str">
+      <c r="S10" s="7">
         <f>IF(Topology!S10=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="T10" s="7" t="str">
         <f>IF(Topology!T10=1,10,"")</f>
@@ -11743,9 +11673,9 @@
         <f>IF(Topology!F11=1,10,"")</f>
         <v/>
       </c>
-      <c r="G11" s="7" t="str">
+      <c r="G11" s="7">
         <f>IF(Topology!G11=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="H11" s="7" t="str">
         <f>IF(Topology!H11=1,10,"")</f>
@@ -11771,9 +11701,9 @@
         <f>IF(Topology!M11=1,10,"")</f>
         <v/>
       </c>
-      <c r="N11" s="7" t="str">
+      <c r="N11" s="7">
         <f>IF(Topology!N11=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="O11" s="7" t="str">
         <f>IF(Topology!O11=1,10,"")</f>
@@ -11787,9 +11717,9 @@
         <f>IF(Topology!Q11=1,10,"")</f>
         <v/>
       </c>
-      <c r="R11" s="7" t="str">
+      <c r="R11" s="7">
         <f>IF(Topology!R11=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="S11" s="7" t="str">
         <f>IF(Topology!S11=1,10,"")</f>
@@ -11847,9 +11777,9 @@
         <f>IF(Topology!I12=1,10,"")</f>
         <v/>
       </c>
-      <c r="J12" s="7" t="str">
+      <c r="J12" s="7">
         <f>IF(Topology!J12=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="K12" s="7" t="str">
         <f>IF(Topology!K12=1,10,"")</f>
@@ -11871,17 +11801,17 @@
         <f>IF(Topology!O12=1,10,"")</f>
         <v/>
       </c>
-      <c r="P12" s="7" t="str">
+      <c r="P12" s="7">
         <f>IF(Topology!P12=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="Q12" s="7" t="str">
         <f>IF(Topology!Q12=1,10,"")</f>
         <v/>
       </c>
-      <c r="R12" s="7" t="str">
+      <c r="R12" s="7">
         <f>IF(Topology!R12=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="S12" s="7" t="str">
         <f>IF(Topology!S12=1,10,"")</f>
@@ -11911,21 +11841,21 @@
       <c r="B13" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="7" t="str">
+      <c r="C13" s="7">
         <f>IF(Topology!C13=1,10,"")</f>
-        <v/>
-      </c>
-      <c r="D13" s="7" t="str">
+        <v>10</v>
+      </c>
+      <c r="D13" s="7">
         <f>IF(Topology!D13=1,10,"")</f>
-        <v/>
-      </c>
-      <c r="E13" s="7" t="str">
+        <v>10</v>
+      </c>
+      <c r="E13" s="7">
         <f>IF(Topology!E13=1,10,"")</f>
-        <v/>
-      </c>
-      <c r="F13" s="7" t="str">
+        <v>10</v>
+      </c>
+      <c r="F13" s="7">
         <f>IF(Topology!F13=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="G13" s="7" t="str">
         <f>IF(Topology!G13=1,10,"")</f>
@@ -12027,17 +11957,17 @@
         <f>IF(Topology!H14=1,10,"")</f>
         <v/>
       </c>
-      <c r="I14" s="7" t="str">
+      <c r="I14" s="7">
         <f>IF(Topology!I14=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="J14" s="7" t="str">
         <f>IF(Topology!J14=1,10,"")</f>
         <v/>
       </c>
-      <c r="K14" s="7" t="str">
+      <c r="K14" s="7">
         <f>IF(Topology!K14=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="L14" s="7" t="str">
         <f>IF(Topology!L14=1,10,"")</f>
@@ -12111,13 +12041,13 @@
         <f>IF(Topology!F15=1,10,"")</f>
         <v/>
       </c>
-      <c r="G15" s="7" t="str">
+      <c r="G15" s="7">
         <f>IF(Topology!G15=1,10,"")</f>
-        <v/>
-      </c>
-      <c r="H15" s="7" t="str">
+        <v>10</v>
+      </c>
+      <c r="H15" s="7">
         <f>IF(Topology!H15=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="I15" s="7" t="str">
         <f>IF(Topology!I15=1,10,"")</f>
@@ -12147,9 +12077,9 @@
         <f>IF(Topology!O15=1,10,"")</f>
         <v/>
       </c>
-      <c r="P15" s="7" t="str">
+      <c r="P15" s="7">
         <f>IF(Topology!P15=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="Q15" s="7" t="str">
         <f>IF(Topology!Q15=1,10,"")</f>
@@ -12223,9 +12153,9 @@
         <f>IF(Topology!K16=1,10,"")</f>
         <v/>
       </c>
-      <c r="L16" s="7" t="str">
+      <c r="L16" s="7">
         <f>IF(Topology!L16=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="M16" s="7" t="str">
         <f>IF(Topology!M16=1,10,"")</f>
@@ -12235,17 +12165,17 @@
         <f>IF(Topology!N16=1,10,"")</f>
         <v/>
       </c>
-      <c r="O16" s="7" t="str">
+      <c r="O16" s="7">
         <f>IF(Topology!O16=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="P16" s="7" t="str">
         <f>IF(Topology!P16=1,10,"")</f>
         <v/>
       </c>
-      <c r="Q16" s="7" t="str">
+      <c r="Q16" s="7">
         <f>IF(Topology!Q16=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="R16" s="7" t="str">
         <f>IF(Topology!R16=1,10,"")</f>
@@ -12295,9 +12225,9 @@
         <f>IF(Topology!F17=1,10,"")</f>
         <v/>
       </c>
-      <c r="G17" s="7" t="str">
+      <c r="G17" s="7">
         <f>IF(Topology!G17=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="H17" s="7" t="str">
         <f>IF(Topology!H17=1,10,"")</f>
@@ -12331,17 +12261,17 @@
         <f>IF(Topology!O17=1,10,"")</f>
         <v/>
       </c>
-      <c r="P17" s="7" t="str">
+      <c r="P17" s="7">
         <f>IF(Topology!P17=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="Q17" s="7" t="str">
         <f>IF(Topology!Q17=1,10,"")</f>
         <v/>
       </c>
-      <c r="R17" s="7" t="str">
+      <c r="R17" s="7">
         <f>IF(Topology!R17=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="S17" s="7" t="str">
         <f>IF(Topology!S17=1,10,"")</f>
@@ -12403,13 +12333,13 @@
         <f>IF(Topology!J18=1,10,"")</f>
         <v/>
       </c>
-      <c r="K18" s="7" t="str">
+      <c r="K18" s="7">
         <f>IF(Topology!K18=1,10,"")</f>
-        <v/>
-      </c>
-      <c r="L18" s="7" t="str">
+        <v>10</v>
+      </c>
+      <c r="L18" s="7">
         <f>IF(Topology!L18=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="M18" s="7" t="str">
         <f>IF(Topology!M18=1,10,"")</f>
@@ -12427,9 +12357,9 @@
         <f>IF(Topology!P18=1,10,"")</f>
         <v/>
       </c>
-      <c r="Q18" s="7" t="str">
+      <c r="Q18" s="7">
         <f>IF(Topology!Q18=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="R18" s="7" t="str">
         <f>IF(Topology!R18=1,10,"")</f>
@@ -12439,9 +12369,9 @@
         <f>IF(Topology!S18=1,10,"")</f>
         <v/>
       </c>
-      <c r="T18" s="7" t="str">
+      <c r="T18" s="7">
         <f>IF(Topology!T18=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="U18" s="7" t="str">
         <f>IF(Topology!U18=1,10,"")</f>
@@ -12491,17 +12421,17 @@
         <f>IF(Topology!I19=1,10,"")</f>
         <v/>
       </c>
-      <c r="J19" s="7" t="str">
+      <c r="J19" s="7">
         <f>IF(Topology!J19=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="K19" s="7" t="str">
         <f>IF(Topology!K19=1,10,"")</f>
         <v/>
       </c>
-      <c r="L19" s="7" t="str">
+      <c r="L19" s="7">
         <f>IF(Topology!L19=1,10,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="M19" s="7" t="str">
         <f>IF(Topology!M19=1,10,"")</f>
@@ -12675,9 +12605,9 @@
         <f>IF(Topology!I21=1,10,"")</f>
         <v>10</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="7" t="str">
         <f>IF(Topology!J21=1,10,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="K21" s="7" t="str">
         <f>IF(Topology!K21=1,10,"")</f>
@@ -12755,21 +12685,21 @@
         <f>IF(Topology!F22=1,10,"")</f>
         <v/>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="7" t="str">
         <f>IF(Topology!G22=1,10,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="H22" s="7">
         <f>IF(Topology!H22=1,10,"")</f>
         <v>10</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="7" t="str">
         <f>IF(Topology!I22=1,10,"")</f>
-        <v>10</v>
-      </c>
-      <c r="J22" s="7">
+        <v/>
+      </c>
+      <c r="J22" s="7" t="str">
         <f>IF(Topology!J22=1,10,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="K22" s="7" t="str">
         <f>IF(Topology!K22=1,10,"")</f>
@@ -12847,17 +12777,17 @@
         <f>IF(Topology!F23=1,10,"")</f>
         <v/>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="8" t="str">
         <f>IF(Topology!G23=1,10,"")</f>
-        <v>10</v>
-      </c>
-      <c r="H23" s="8">
+        <v/>
+      </c>
+      <c r="H23" s="8" t="str">
         <f>IF(Topology!H23=1,10,"")</f>
-        <v>10</v>
-      </c>
-      <c r="I23" s="8">
+        <v/>
+      </c>
+      <c r="I23" s="8" t="str">
         <f>IF(Topology!I23=1,10,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="J23" s="8">
         <f>IF(Topology!J23=1,10,"")</f>
@@ -13291,9 +13221,9 @@
       <c r="B28" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="7" t="str">
         <f>IF(Topology!C28=1,10,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="D28" s="7" t="str">
         <f>IF(Topology!D28=1,10,"")</f>
@@ -13383,9 +13313,9 @@
       <c r="B29" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="7" t="str">
         <f>IF(Topology!C29=1,10,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="D29" s="7" t="str">
         <f>IF(Topology!D29=1,10,"")</f>
@@ -13475,9 +13405,9 @@
       <c r="B30" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="7" t="str">
         <f>IF(Topology!C30=1,10,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="D30" s="7" t="str">
         <f>IF(Topology!D30=1,10,"")</f>
@@ -13567,9 +13497,9 @@
       <c r="B31" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="7" t="str">
         <f>IF(Topology!C31=1,10,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="D31" s="7" t="str">
         <f>IF(Topology!D31=1,10,"")</f>
@@ -14043,21 +13973,21 @@
         <f>IF(Topology!F36=1,10,"")</f>
         <v/>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="7" t="str">
         <f>IF(Topology!G36=1,10,"")</f>
-        <v>10</v>
-      </c>
-      <c r="H36" s="7">
+        <v/>
+      </c>
+      <c r="H36" s="7" t="str">
         <f>IF(Topology!H36=1,10,"")</f>
-        <v>10</v>
-      </c>
-      <c r="I36" s="7">
+        <v/>
+      </c>
+      <c r="I36" s="7" t="str">
         <f>IF(Topology!I36=1,10,"")</f>
-        <v>10</v>
-      </c>
-      <c r="J36" s="7">
+        <v/>
+      </c>
+      <c r="J36" s="7" t="str">
         <f>IF(Topology!J36=1,10,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="K36" s="7" t="str">
         <f>IF(Topology!K36=1,10,"")</f>
@@ -14135,21 +14065,21 @@
         <f>IF(Topology!F37=1,10,"")</f>
         <v/>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="7" t="str">
         <f>IF(Topology!G37=1,10,"")</f>
-        <v>10</v>
-      </c>
-      <c r="H37" s="7">
+        <v/>
+      </c>
+      <c r="H37" s="7" t="str">
         <f>IF(Topology!H37=1,10,"")</f>
-        <v>10</v>
-      </c>
-      <c r="I37" s="7">
+        <v/>
+      </c>
+      <c r="I37" s="7" t="str">
         <f>IF(Topology!I37=1,10,"")</f>
-        <v>10</v>
-      </c>
-      <c r="J37" s="7">
+        <v/>
+      </c>
+      <c r="J37" s="7" t="str">
         <f>IF(Topology!J37=1,10,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="K37" s="7" t="str">
         <f>IF(Topology!K37=1,10,"")</f>
@@ -14227,21 +14157,21 @@
         <f>IF(Topology!F38=1,10,"")</f>
         <v/>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="8" t="str">
         <f>IF(Topology!G38=1,10,"")</f>
-        <v>10</v>
-      </c>
-      <c r="H38" s="8">
+        <v/>
+      </c>
+      <c r="H38" s="8" t="str">
         <f>IF(Topology!H38=1,10,"")</f>
-        <v>10</v>
-      </c>
-      <c r="I38" s="8">
+        <v/>
+      </c>
+      <c r="I38" s="8" t="str">
         <f>IF(Topology!I38=1,10,"")</f>
-        <v>10</v>
-      </c>
-      <c r="J38" s="8">
+        <v/>
+      </c>
+      <c r="J38" s="8" t="str">
         <f>IF(Topology!J38=1,10,"")</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="K38" s="8" t="str">
         <f>IF(Topology!K38=1,10,"")</f>
@@ -14302,12 +14232,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81EF4E1D-6CE0-4F02-8B9E-F2818C0A814C}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -14608,7 +14538,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -15406,7 +15336,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -15424,7 +15354,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>